<commit_message>
implemented download for spreadsheet and pdf
</commit_message>
<xml_diff>
--- a/app/public/templates/template-parameter-logs.xlsx
+++ b/app/public/templates/template-parameter-logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\water-monitoring-system\app\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D397F886-2015-44A3-B583-03D8F3568A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DE89CB-FCDC-4E91-92B6-9B8074B3FAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{68FBDC9F-33A5-487F-9B7D-1FC223F0A2D2}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="18000" windowHeight="9360" xr2:uid="{68FBDC9F-33A5-487F-9B7D-1FC223F0A2D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,21 +36,9 @@
     <t>{parameter}</t>
   </si>
   <si>
-    <t>{parameter} Range</t>
-  </si>
-  <si>
     <t>{pond name} water {paramter} logs</t>
   </si>
   <si>
-    <t>average {parameter}</t>
-  </si>
-  <si>
-    <t>mean rate of change</t>
-  </si>
-  <si>
-    <t>hourly average</t>
-  </si>
-  <si>
     <t>{date}</t>
   </si>
   <si>
@@ -63,22 +51,34 @@
     <t>B8 range</t>
   </si>
   <si>
-    <t>B9 average</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> B10 mean rate of change</t>
-  </si>
-  <si>
-    <t>B11 hourly average</t>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>B9 mean</t>
+  </si>
+  <si>
+    <t>B11 mean rate of change</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B10 std derv</t>
+  </si>
+  <si>
+    <t>A14 {date}</t>
+  </si>
+  <si>
+    <t>B14 {time h:mm a}</t>
   </si>
   <si>
     <t>C14 {value} {unit}</t>
   </si>
   <si>
-    <t>B14 {time h:mm a}</t>
-  </si>
-  <si>
-    <t>A14 {date}</t>
+    <t>Mean rate of change</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Range</t>
   </si>
 </sst>
 </file>
@@ -138,20 +138,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -585,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A8C91A7-60CC-4E0F-BD6B-D23CB1E9DABB}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,83 +600,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="4" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>